<commit_message>
adding may budget to excel file
changes to comment
</commit_message>
<xml_diff>
--- a/budget.xlsx
+++ b/budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User1\Documents\GitHub\myofficegit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC96F941-8377-4A90-B2E4-80857DB92FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A97CD1-3775-4909-9B2B-AD01C0074FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5535" yWindow="675" windowWidth="14385" windowHeight="14805" xr2:uid="{A49D5F1C-227A-4385-A859-3518DD97DFB2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Month</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>March</t>
+  </si>
+  <si>
+    <t>May</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3228A0B5-A6A9-4F55-BC13-A690FBC8E2CB}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,6 +481,14 @@
         <v>3434</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>7666</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>